<commit_message>
fix remove isscaap bug in figures
</commit_message>
<xml_diff>
--- a/output/aggregate_tables/top10species_by_area.xlsx
+++ b/output/aggregate_tables/top10species_by_area.xlsx
@@ -49,9 +49,6 @@
     <t>Arctica islandica</t>
   </si>
   <si>
-    <t>Pagophilus groenlandicus</t>
-  </si>
-  <si>
     <t>Chionoecetes opilio</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
     <t>Spisula solidissima</t>
   </si>
   <si>
+    <t>Crassostrea virginica</t>
+  </si>
+  <si>
     <t>Micromesistius poutassou</t>
   </si>
   <si>
@@ -88,7 +88,7 @@
     <t>Mallotus villosus</t>
   </si>
   <si>
-    <t>Laminaria hyperborea</t>
+    <t>Sebastes mentella</t>
   </si>
   <si>
     <t>Brevoortia patronus</t>
@@ -361,10 +361,10 @@
     <t>Strangomera bentincki</t>
   </si>
   <si>
-    <t>Lessonia nigrescens</t>
-  </si>
-  <si>
     <t>Sarda chiliensis</t>
+  </si>
+  <si>
+    <t>Merluccius gayi</t>
   </si>
   <si>
     <t>Euphausia superba</t>
@@ -811,7 +811,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>81425</v>
+        <v>80249.2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -819,7 +819,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>80249.2</v>
+        <v>73585.92</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -827,7 +827,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>73585.92</v>
+        <v>66899.18000000001</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -835,7 +835,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>66899.18000000001</v>
+        <v>60674.75</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -843,7 +843,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>60674.75</v>
+        <v>47148.78</v>
       </c>
     </row>
   </sheetData>
@@ -1422,26 +1422,26 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>28</v>
       </c>
       <c r="B8">
-        <v>197088.22</v>
+        <v>117107.95</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B9">
-        <v>117107.95</v>
+        <v>100798.73</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>110</v>
       </c>
       <c r="B10">
-        <v>100798.73</v>
+        <v>94502.89999999999</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1449,7 +1449,7 @@
         <v>111</v>
       </c>
       <c r="B11">
-        <v>94502.89999999999</v>
+        <v>87525.53</v>
       </c>
     </row>
   </sheetData>
@@ -1576,7 +1576,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>1554603.6</v>
@@ -1651,7 +1651,7 @@
         <v>19</v>
       </c>
       <c r="B11">
-        <v>162027.69</v>
+        <v>94462.19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>